<commit_message>
Added files - 4th Mar
</commit_message>
<xml_diff>
--- a/Columnar Transposition.xlsx
+++ b/Columnar Transposition.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ravi\Masters\Spring 2023\23S-CPEG672-610\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ravi\Masters\Spring 2023\23S-CPEG672-610\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B283521-C598-4FD7-BA27-6573B09755C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E706FE1A-B247-4571-B579-8255E0E8CDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{39E3B8F2-E722-4221-8B73-203A514AE0EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="25">
   <si>
     <t>mrlsehdsolmmnoilvtelonraesdieuntuetearbfuadeerifeoenultmiemitnnltspttahinneesyumtetaauietoieehematytodcntdlsooaresogrsasnlrspsgnletssocasdtholhhlasiguueonrrserhtirnstslsynrptmienmnrtemundtouoiteslmnuwadtrptieeitgadnayasrdesimtedthgyutpeeurveanmasuomheahmbuamdfweeueognenaatcerisacevrsfsiiayentndteiiretsnfonretotfohehidptfenootrsohodbstansitgennwrrmfeshveoibueldtvrraanwetoanweeaftealcyssdtlgvnanetufwfehmtsatfsraitrhdirsfuosliwiydhisruntiyemeiertnmasvlotimmnewvttedheotdtpytdlwetohrafdthstrnartefocpnoisehnpifoanunrunilyrenomrbdefuwatulowentospaooirshoouefdetandnthonceeoesectaexfslrdtahiaensgoahugy</t>
   </si>
@@ -112,84 +111,6 @@
   </si>
   <si>
     <t>no of col</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -2876,233 +2797,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{253E3FC3-ECB2-4DF8-B00E-F95F76EE8AE7}">
-  <dimension ref="A1:Z14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="26" width="8.7109375" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3">
-        <v>8</v>
-      </c>
-      <c r="J2" s="3">
-        <v>9</v>
-      </c>
-      <c r="K2" s="3">
-        <v>10</v>
-      </c>
-      <c r="L2" s="3">
-        <v>11</v>
-      </c>
-      <c r="M2" s="3">
-        <v>12</v>
-      </c>
-      <c r="N2" s="3">
-        <v>13</v>
-      </c>
-      <c r="O2" s="3">
-        <v>14</v>
-      </c>
-      <c r="P2" s="3">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>16</v>
-      </c>
-      <c r="R2" s="3">
-        <v>17</v>
-      </c>
-      <c r="S2" s="3">
-        <v>18</v>
-      </c>
-      <c r="T2" s="3">
-        <v>19</v>
-      </c>
-      <c r="U2" s="3">
-        <v>20</v>
-      </c>
-      <c r="V2" s="3">
-        <v>21</v>
-      </c>
-      <c r="W2" s="3">
-        <v>22</v>
-      </c>
-      <c r="X2" s="3">
-        <v>23</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>24</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <f>-1866</f>
-        <v>-1866</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4683</v>
-      </c>
-      <c r="C5" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <f>-3297</f>
-        <v>-3297</v>
-      </c>
-      <c r="B6" s="1">
-        <v>4956</v>
-      </c>
-      <c r="C6" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C10" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>52710</v>
-      </c>
-      <c r="C11" s="1">
-        <v>8</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>41052</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>18732</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>